<commit_message>
implemented filtered recording, i think. also started making the learning ai smarter
</commit_message>
<xml_diff>
--- a/analysis/initial_card_analysis.xlsx
+++ b/analysis/initial_card_analysis.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="746" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="814" uniqueCount="223">
   <si>
     <t>Keywords</t>
   </si>
@@ -665,6 +665,27 @@
   </si>
   <si>
     <t>Max Depreciation Lifetime Cost</t>
+  </si>
+  <si>
+    <t>Hybrid</t>
+  </si>
+  <si>
+    <t>Count</t>
+  </si>
+  <si>
+    <t>Lifetime Cost</t>
+  </si>
+  <si>
+    <t>Lifetime Action Cost</t>
+  </si>
+  <si>
+    <t>Lifetime Action Efficiency</t>
+  </si>
+  <si>
+    <t>Front Load Companion Cost</t>
+  </si>
+  <si>
+    <t>Lifetime Companion Efficiency</t>
   </si>
 </sst>
 </file>
@@ -739,9 +760,13 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -767,15 +792,16 @@
   </sheetPr>
   <dimension ref="A1:AZ120"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="4" ySplit="0" topLeftCell="T1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topRight" activeCell="U9" activeCellId="1" sqref="H2:N2 U9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.280612244898"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.9030612244898"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.6530612244898"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="11.5204081632653"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.7959183673469"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.7397959183673"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.0459183673469"/>
@@ -16251,7 +16277,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+      <selection pane="topLeft" activeCell="D3" activeCellId="1" sqref="H2:N2 D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -16355,15 +16381,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:N26"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2:N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="7" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.6530612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16371,15 +16399,1047 @@
         <v>205</v>
       </c>
       <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="I1" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>213</v>
       </c>
+      <c r="B2" s="0" t="s">
+        <v>217</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>218</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>214</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>219</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>220</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>213</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>214</v>
+      </c>
+      <c r="J2" s="0" t="s">
+        <v>221</v>
+      </c>
+      <c r="K2" s="0" t="s">
+        <v>219</v>
+      </c>
+      <c r="L2" s="0" t="s">
+        <v>218</v>
+      </c>
+      <c r="M2" s="0" t="s">
+        <v>220</v>
+      </c>
+      <c r="N2" s="0" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="I3" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="J3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="K3" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="L3" s="0" t="n">
+        <v>56</v>
+      </c>
+      <c r="M3" s="0" t="n">
+        <v>5.09</v>
+      </c>
+      <c r="N3" s="0" t="n">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="I4" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="J4" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="K4" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="L4" s="0" t="n">
+        <v>49</v>
+      </c>
+      <c r="M4" s="0" t="n">
+        <v>4.45</v>
+      </c>
+      <c r="N4" s="0" t="n">
+        <v>24.5</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="I5" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="J5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K5" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="L5" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="M5" s="0" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="N5" s="0" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="I6" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="J6" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="K6" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="L6" s="0" t="n">
+        <v>49</v>
+      </c>
+      <c r="M6" s="0" t="n">
+        <v>4.45</v>
+      </c>
+      <c r="N6" s="0" t="n">
+        <v>24.5</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="I7" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="J7" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="K7" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="L7" s="0" t="n">
+        <v>70</v>
+      </c>
+      <c r="M7" s="0" t="n">
+        <v>6.36</v>
+      </c>
+      <c r="N7" s="0" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="I8" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="J8" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K8" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="L8" s="0" t="n">
+        <v>49</v>
+      </c>
+      <c r="M8" s="0" t="n">
+        <v>4.9</v>
+      </c>
+      <c r="N8" s="0" t="n">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="I9" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="J9" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="K9" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="L9" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="M9" s="0" t="n">
+        <v>3.82</v>
+      </c>
+      <c r="N9" s="0" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E10" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H10" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="I10" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="J10" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K10" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="L10" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="M10" s="0" t="n">
+        <v>2.8</v>
+      </c>
+      <c r="N10" s="0" t="n">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E11" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H11" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="I11" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="J11" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="K11" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="L11" s="0" t="n">
+        <v>63</v>
+      </c>
+      <c r="M11" s="0" t="n">
+        <v>5.25</v>
+      </c>
+      <c r="N11" s="0" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="B12" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D12" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E12" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F12" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H12" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="I12" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="J12" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K12" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="L12" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="M12" s="0" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="N12" s="0" t="n">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="B13" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E13" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F13" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H13" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="I13" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="J13" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="K13" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="L13" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="M13" s="0" t="n">
+        <v>3.82</v>
+      </c>
+      <c r="N13" s="0" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="B14" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="D14" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E14" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F14" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="H14" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="I14" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="J14" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K14" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="L14" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="M14" s="0" t="n">
+        <v>3.33</v>
+      </c>
+      <c r="N14" s="0" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="B15" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C15" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="D15" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E15" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F15" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="H15" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="I15" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="J15" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K15" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="L15" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="M15" s="0" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="N15" s="0" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="B16" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C16" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D16" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E16" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F16" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H16" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="I16" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="J16" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K16" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="L16" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="M16" s="0" t="n">
+        <v>3.14</v>
+      </c>
+      <c r="N16" s="0" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="B17" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C17" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D17" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E17" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F17" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H17" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="I17" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="J17" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="K17" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="L17" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="M17" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="N17" s="0" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="B18" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C18" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="D18" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E18" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F18" s="0" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="H18" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="I18" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="J18" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="K18" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="L18" s="0" t="n">
+        <v>53</v>
+      </c>
+      <c r="M18" s="0" t="n">
+        <v>5.89</v>
+      </c>
+      <c r="N18" s="0" t="n">
+        <v>26.5</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="B19" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C19" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="D19" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E19" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F19" s="0" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="H19" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="I19" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="J19" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K19" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="L19" s="0" t="n">
+        <v>39</v>
+      </c>
+      <c r="M19" s="0" t="n">
+        <v>4.33</v>
+      </c>
+      <c r="N19" s="0" t="n">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="B20" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C20" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="D20" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E20" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F20" s="0" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="H20" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="I20" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="J20" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K20" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="L20" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="M20" s="0" t="n">
+        <v>3.83</v>
+      </c>
+      <c r="N20" s="0" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="B21" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C21" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="D21" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E21" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F21" s="0" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="H21" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="I21" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="J21" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K21" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="L21" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="M21" s="0" t="n">
+        <v>2.83</v>
+      </c>
+      <c r="N21" s="0" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="B22" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C22" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="D22" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E22" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F22" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="H22" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="I22" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="J22" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K22" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="L22" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="M22" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="N22" s="0" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="B23" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C23" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D23" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E23" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F23" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H23" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="I23" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="J23" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K23" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="L23" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="M23" s="0" t="n">
+        <v>3.56</v>
+      </c>
+      <c r="N23" s="0" t="n">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="B24" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C24" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="D24" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E24" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F24" s="0" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="H24" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="I24" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="J24" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K24" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="L24" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="M24" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="N24" s="0" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="B25" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C25" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="D25" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E25" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F25" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="H25" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="I25" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="J25" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K25" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="L25" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="M25" s="0" t="n">
+        <v>3.62</v>
+      </c>
+      <c r="N25" s="0" t="n">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="B26" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C26" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="D26" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E26" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F26" s="0" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="H26" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="I26" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="J26" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K26" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="L26" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="M26" s="0" t="n">
+        <v>3.57</v>
+      </c>
+      <c r="N26" s="0" t="n">
+        <v>25</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B1:C1"/>
+  <mergeCells count="2">
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="I1:N1"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>